<commit_message>
add lucro 3un. 5un. 10un.
</commit_message>
<xml_diff>
--- a/Cadastro e Preço.xlsx
+++ b/Cadastro e Preço.xlsx
@@ -532,7 +532,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,6 +571,21 @@
           <t>Lucro</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Lucro 3un.</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Lucro 5un.</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Lucro 10un.</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -593,6 +608,15 @@
       <c r="F2" t="n">
         <v>17.11</v>
       </c>
+      <c r="G2" t="n">
+        <v>51.33</v>
+      </c>
+      <c r="H2" t="n">
+        <v>85.55</v>
+      </c>
+      <c r="I2" t="n">
+        <v>171.1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -615,6 +639,15 @@
       <c r="F3" t="n">
         <v>16.25</v>
       </c>
+      <c r="G3" t="n">
+        <v>48.75</v>
+      </c>
+      <c r="H3" t="n">
+        <v>81.25</v>
+      </c>
+      <c r="I3" t="n">
+        <v>162.5</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -637,6 +670,15 @@
       <c r="F4" t="n">
         <v>18.83</v>
       </c>
+      <c r="G4" t="n">
+        <v>56.48999999999999</v>
+      </c>
+      <c r="H4" t="n">
+        <v>94.14999999999999</v>
+      </c>
+      <c r="I4" t="n">
+        <v>188.3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -658,6 +700,15 @@
       </c>
       <c r="F5" t="n">
         <v>17.97</v>
+      </c>
+      <c r="G5" t="n">
+        <v>53.91</v>
+      </c>
+      <c r="H5" t="n">
+        <v>89.84999999999999</v>
+      </c>
+      <c r="I5" t="n">
+        <v>179.7</v>
       </c>
     </row>
   </sheetData>
@@ -671,7 +722,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -710,6 +761,21 @@
           <t>Lucro</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Lucro 3un.</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Lucro 5un.</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Lucro 10un.</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -732,6 +798,15 @@
       <c r="F2" t="n">
         <v>15.72</v>
       </c>
+      <c r="G2" t="n">
+        <v>47.16</v>
+      </c>
+      <c r="H2" t="n">
+        <v>78.60000000000001</v>
+      </c>
+      <c r="I2" t="n">
+        <v>157.2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -754,6 +829,15 @@
       <c r="F3" t="n">
         <v>14.93</v>
       </c>
+      <c r="G3" t="n">
+        <v>44.79</v>
+      </c>
+      <c r="H3" t="n">
+        <v>74.65000000000001</v>
+      </c>
+      <c r="I3" t="n">
+        <v>149.3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -776,6 +860,15 @@
       <c r="F4" t="n">
         <v>17.3</v>
       </c>
+      <c r="G4" t="n">
+        <v>51.90000000000001</v>
+      </c>
+      <c r="H4" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>173</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -797,6 +890,15 @@
       </c>
       <c r="F5" t="n">
         <v>16.51</v>
+      </c>
+      <c r="G5" t="n">
+        <v>49.53</v>
+      </c>
+      <c r="H5" t="n">
+        <v>82.55000000000001</v>
+      </c>
+      <c r="I5" t="n">
+        <v>165.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>